<commit_message>
chore(env): migrate project to Python 3.12 for OpenCV compatibility
</commit_message>
<xml_diff>
--- a/excel_templates/express_import_template.xlsx
+++ b/excel_templates/express_import_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://edsth-my.sharepoint.com/personal/piyaphon_w_eds_co_th/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyaphon.w\Documents\Projects\ExpressAutomation\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC1048E6D95D72AE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B09755C-4640-48F1-9D43-500120BD07BA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5577D2D2-4F83-486D-9DD2-739AA5EA5179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23760" yWindow="1785" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,20 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Department</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>MBK</t>
   </si>
   <si>
@@ -48,24 +39,38 @@
     <t>001</t>
   </si>
   <si>
-    <t>BillNumber</t>
-  </si>
-  <si>
-    <t>ProductCode</t>
-  </si>
-  <si>
-    <t>PricePerUnit</t>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Dept</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>UnitCost</t>
+  </si>
+  <si>
+    <t>01/10/68</t>
+  </si>
+  <si>
+    <t>6500116099</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +81,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,13 +113,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -390,71 +398,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>244258</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5">
-        <v>6500116081</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
         <v>9910.57</v>
       </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" twoDigitTextYear="1"/>
+    <ignoredError sqref="E2 C2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(express_excel_entry): add full Excel data entry workflow with Alt+A for new entry
</commit_message>
<xml_diff>
--- a/excel_templates/express_import_template.xlsx
+++ b/excel_templates/express_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyaphon.w\Documents\Projects\ExpressAutomation\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5577D2D2-4F83-486D-9DD2-739AA5EA5179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A44E851-D78A-4EF8-A7DE-F80C3D7D6DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -60,7 +60,13 @@
     <t>01/10/68</t>
   </si>
   <si>
-    <t>6500116099</t>
+    <t xml:space="preserve"> 1.00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,350.00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22,495.82 </t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,7 +415,7 @@
     <col min="1" max="1" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -449,31 +455,45 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
+      <c r="D2">
+        <v>6500118082</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>9910.57</v>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>6500118083</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2" twoDigitTextYear="1"/>
-    <ignoredError sqref="E2 C2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update after git pull
</commit_message>
<xml_diff>
--- a/excel_templates/express_import_template.xlsx
+++ b/excel_templates/express_import_template.xlsx
@@ -5,31 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyaphon.w\Documents\Projects\ExpressAutomation\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://edsth-my.sharepoint.com/personal/piyaphon_w_eds_co_th/Documents/Desktop/New folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33AB4CE-B276-4A2B-96C4-F8EC3A6B9336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{5A44E851-D78A-4EF8-A7DE-F80C3D7D6DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F34004E1-A6F1-4C48-96A3-A77585EFA0B4}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -467,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>6500118084</v>
+        <v>6500118090</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
@@ -490,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>6500118085</v>
+        <v>6500118091</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>

</xml_diff>